<commit_message>
adds province, graticule, and engine models. adds json and xml formats. fixes bug with assigning Admin roles. adds minor reformating to panel index views
</commit_message>
<xml_diff>
--- a/public/Database.template.xlsx
+++ b/public/Database.template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-80" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="807">
   <si>
     <t>Form A</t>
   </si>
@@ -2442,6 +2442,9 @@
   </si>
   <si>
     <t>Gracillia spp</t>
+  </si>
+  <si>
+    <t>Graticule</t>
   </si>
 </sst>
 </file>
@@ -3333,8 +3336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3359,7 +3362,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>11</v>
+        <v>806</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>13</v>
@@ -4390,10 +4393,7 @@
       <c r="P51" s="9"/>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E50">
-      <formula1>"long-tail,outboard,inboard"</formula1>
-    </dataValidation>
+  <dataValidations count="8">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F51 K2:K51">
       <formula1>0</formula1>
       <formula2>1000</formula2>
@@ -4416,6 +4416,12 @@
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P51">
       <formula1>0</formula1>
       <formula2>100000000</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E51">
+      <formula1>"OB,LT,IB"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G51">
+      <formula1>"1234,2345"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6507,7 +6513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3451"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes excel file import functions. updates supervisor dashboard. links surveyors to landings. updates template files
</commit_message>
<xml_diff>
--- a/public/Database.template.xlsx
+++ b/public/Database.template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="C470" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="10900" yWindow="660" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="840">
   <si>
     <t>Form A</t>
   </si>
@@ -2478,15 +2478,6 @@
     <t>Tanah Ampo</t>
   </si>
   <si>
-    <t>Anantelo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ahmad </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gemelut </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bunutun </t>
   </si>
   <si>
@@ -2496,9 +2487,6 @@
     <t xml:space="preserve">Kusamba </t>
   </si>
   <si>
-    <t>Pessinggahan</t>
-  </si>
-  <si>
     <t>Candidasa</t>
   </si>
   <si>
@@ -2533,6 +2521,33 @@
   </si>
   <si>
     <t>Fleet No.</t>
+  </si>
+  <si>
+    <t>No. vessels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jemelut </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amed </t>
+  </si>
+  <si>
+    <t>Angantelo</t>
+  </si>
+  <si>
+    <t>Pesinggahan</t>
+  </si>
+  <si>
+    <t>Dep. Date</t>
+  </si>
+  <si>
+    <t>Abort (Y/N)</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>Conditions</t>
   </si>
 </sst>
 </file>
@@ -2540,7 +2555,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -3068,7 +3083,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3077,12 +3092,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyBorder="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyBorder="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3197,15 +3216,35 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="7"/>
     <cellStyle name="Normal 3" xfId="9"/>
@@ -3608,7 +3647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -3782,10 +3821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="56.5" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3812,7 +3851,7 @@
       <c r="A3" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:3" s="33" customFormat="1" ht="28" customHeight="1">
@@ -3831,32 +3870,39 @@
     </row>
     <row r="6" spans="1:3" s="33" customFormat="1" ht="28" customHeight="1">
       <c r="A6" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="41"/>
+        <v>831</v>
+      </c>
+      <c r="B6" s="53"/>
       <c r="C6" s="34"/>
     </row>
     <row r="7" spans="1:3" s="33" customFormat="1" ht="28" customHeight="1">
       <c r="A7" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="41"/>
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="1:3" s="33" customFormat="1" ht="28" customHeight="1" thickBot="1">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:3" s="33" customFormat="1" ht="28" customHeight="1">
+      <c r="A8" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="34"/>
+    </row>
+    <row r="9" spans="1:3" s="33" customFormat="1" ht="28" customHeight="1" thickBot="1">
+      <c r="A9" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="34"/>
-    </row>
-    <row r="9" spans="1:3" ht="14" thickTop="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="34"/>
+    </row>
+    <row r="10" spans="1:3" ht="14" thickTop="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="date" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the date on which this survey was conducted." sqref="B3">
       <formula1>40909</formula1>
       <formula2>55153</formula2>
@@ -3868,6 +3914,10 @@
     <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the end time for this survey, which must be after the start time." sqref="B5">
       <formula1>B4</formula1>
       <formula2>0.999305555555556</formula2>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the end time for this survey, which must be after the start time." sqref="B6">
+      <formula1>0</formula1>
+      <formula2>9999</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3898,21 +3948,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" thickBottom="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="10.83203125" style="16"/>
-    <col min="9" max="9" width="15.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="16"/>
+    <col min="2" max="9" width="10.83203125" style="16"/>
+    <col min="10" max="10" width="15.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickTop="1" thickBot="1">
+    <row r="1" spans="1:23" ht="15" thickTop="1" thickBot="1">
       <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
@@ -3935,41 +3985,53 @@
         <v>34</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="I1" s="20" t="s">
+        <v>836</v>
+      </c>
+      <c r="J1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="L1" s="20" t="s">
+        <v>837</v>
+      </c>
+      <c r="M1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="N1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="O1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="Q1" s="20" t="s">
+        <v>838</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>839</v>
+      </c>
+      <c r="S1" s="20" t="s">
         <v>805</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="U1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="17"/>
-    </row>
-    <row r="2" spans="1:19" thickBot="1">
+      <c r="W1" s="17"/>
+    </row>
+    <row r="2" spans="1:23" thickBot="1">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3980,19 +4042,23 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
       <c r="M2" s="24"/>
       <c r="N2" s="24"/>
       <c r="O2" s="24"/>
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="17"/>
-    </row>
-    <row r="3" spans="1:19" thickBot="1">
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="17"/>
+    </row>
+    <row r="3" spans="1:23" thickBot="1">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -4003,19 +4069,23 @@
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
       <c r="M3" s="24"/>
       <c r="N3" s="24"/>
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="17"/>
-    </row>
-    <row r="4" spans="1:19" thickBot="1">
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="17"/>
+    </row>
+    <row r="4" spans="1:23" thickBot="1">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -4026,19 +4096,23 @@
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
       <c r="M4" s="24"/>
       <c r="N4" s="24"/>
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
       <c r="Q4" s="24"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="17"/>
-    </row>
-    <row r="5" spans="1:19" thickBot="1">
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="17"/>
+    </row>
+    <row r="5" spans="1:23" thickBot="1">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -4049,7 +4123,7 @@
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
+      <c r="I5" s="54"/>
       <c r="J5" s="24"/>
       <c r="K5" s="24"/>
       <c r="L5" s="24"/>
@@ -4058,10 +4132,14 @@
       <c r="O5" s="24"/>
       <c r="P5" s="24"/>
       <c r="Q5" s="24"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="17"/>
-    </row>
-    <row r="6" spans="1:19" thickBot="1">
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="17"/>
+    </row>
+    <row r="6" spans="1:23" thickBot="1">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -4072,7 +4150,7 @@
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
+      <c r="I6" s="54"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
       <c r="L6" s="24"/>
@@ -4081,10 +4159,14 @@
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
       <c r="Q6" s="24"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="17"/>
-    </row>
-    <row r="7" spans="1:19" thickBot="1">
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="17"/>
+    </row>
+    <row r="7" spans="1:23" thickBot="1">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -4095,7 +4177,7 @@
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="I7" s="54"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
@@ -4104,10 +4186,14 @@
       <c r="O7" s="24"/>
       <c r="P7" s="24"/>
       <c r="Q7" s="24"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="17"/>
-    </row>
-    <row r="8" spans="1:19" thickBot="1">
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="17"/>
+    </row>
+    <row r="8" spans="1:23" thickBot="1">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -4118,7 +4204,7 @@
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="I8" s="54"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
@@ -4127,10 +4213,14 @@
       <c r="O8" s="24"/>
       <c r="P8" s="24"/>
       <c r="Q8" s="24"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="17"/>
-    </row>
-    <row r="9" spans="1:19" thickBot="1">
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="17"/>
+    </row>
+    <row r="9" spans="1:23" thickBot="1">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -4141,7 +4231,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
+      <c r="I9" s="54"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
@@ -4150,10 +4240,14 @@
       <c r="O9" s="24"/>
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="17"/>
-    </row>
-    <row r="10" spans="1:19" thickBot="1">
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="17"/>
+    </row>
+    <row r="10" spans="1:23" thickBot="1">
       <c r="A10" s="22">
         <v>9</v>
       </c>
@@ -4164,7 +4258,7 @@
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
+      <c r="I10" s="54"/>
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
@@ -4173,10 +4267,14 @@
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="17"/>
-    </row>
-    <row r="11" spans="1:19" thickBot="1">
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="17"/>
+    </row>
+    <row r="11" spans="1:23" thickBot="1">
       <c r="A11" s="22">
         <v>10</v>
       </c>
@@ -4187,7 +4285,7 @@
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
+      <c r="I11" s="54"/>
       <c r="J11" s="24"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
@@ -4196,10 +4294,14 @@
       <c r="O11" s="24"/>
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="17"/>
-    </row>
-    <row r="12" spans="1:19" thickBot="1">
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="17"/>
+    </row>
+    <row r="12" spans="1:23" thickBot="1">
       <c r="A12" s="22">
         <v>11</v>
       </c>
@@ -4210,7 +4312,7 @@
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="I12" s="54"/>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
@@ -4219,10 +4321,14 @@
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="17"/>
-    </row>
-    <row r="13" spans="1:19" thickBot="1">
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="17"/>
+    </row>
+    <row r="13" spans="1:23" thickBot="1">
       <c r="A13" s="22">
         <v>12</v>
       </c>
@@ -4233,7 +4339,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="I13" s="54"/>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
@@ -4242,10 +4348,14 @@
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="17"/>
-    </row>
-    <row r="14" spans="1:19" thickBot="1">
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="17"/>
+    </row>
+    <row r="14" spans="1:23" thickBot="1">
       <c r="A14" s="22">
         <v>13</v>
       </c>
@@ -4256,7 +4366,7 @@
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="I14" s="54"/>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
@@ -4265,10 +4375,14 @@
       <c r="O14" s="24"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="17"/>
-    </row>
-    <row r="15" spans="1:19" thickBot="1">
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="17"/>
+    </row>
+    <row r="15" spans="1:23" thickBot="1">
       <c r="A15" s="22">
         <v>14</v>
       </c>
@@ -4279,7 +4393,7 @@
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
+      <c r="I15" s="54"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
@@ -4288,10 +4402,14 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="17"/>
-    </row>
-    <row r="16" spans="1:19" thickBot="1">
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="17"/>
+    </row>
+    <row r="16" spans="1:23" thickBot="1">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -4302,7 +4420,7 @@
       <c r="F16" s="24"/>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
+      <c r="I16" s="54"/>
       <c r="J16" s="24"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
@@ -4311,10 +4429,14 @@
       <c r="O16" s="24"/>
       <c r="P16" s="24"/>
       <c r="Q16" s="24"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="17"/>
-    </row>
-    <row r="17" spans="1:19" thickBot="1">
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="17"/>
+    </row>
+    <row r="17" spans="1:23" thickBot="1">
       <c r="A17" s="22">
         <v>16</v>
       </c>
@@ -4325,7 +4447,7 @@
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="24"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
@@ -4334,10 +4456,14 @@
       <c r="O17" s="24"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="17"/>
-    </row>
-    <row r="18" spans="1:19" thickBot="1">
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="17"/>
+    </row>
+    <row r="18" spans="1:23" thickBot="1">
       <c r="A18" s="22">
         <v>17</v>
       </c>
@@ -4348,7 +4474,7 @@
       <c r="F18" s="24"/>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
+      <c r="I18" s="54"/>
       <c r="J18" s="24"/>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
@@ -4357,10 +4483,14 @@
       <c r="O18" s="24"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="17"/>
-    </row>
-    <row r="19" spans="1:19" thickBot="1">
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="17"/>
+    </row>
+    <row r="19" spans="1:23" thickBot="1">
       <c r="A19" s="22">
         <v>18</v>
       </c>
@@ -4371,7 +4501,7 @@
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
+      <c r="I19" s="54"/>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
@@ -4380,10 +4510,14 @@
       <c r="O19" s="24"/>
       <c r="P19" s="24"/>
       <c r="Q19" s="24"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="17"/>
-    </row>
-    <row r="20" spans="1:19" thickBot="1">
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="25"/>
+      <c r="W19" s="17"/>
+    </row>
+    <row r="20" spans="1:23" thickBot="1">
       <c r="A20" s="22">
         <v>19</v>
       </c>
@@ -4394,7 +4528,7 @@
       <c r="F20" s="24"/>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
+      <c r="I20" s="54"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
@@ -4403,10 +4537,14 @@
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="17"/>
-    </row>
-    <row r="21" spans="1:19" thickBot="1">
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="17"/>
+    </row>
+    <row r="21" spans="1:23" thickBot="1">
       <c r="A21" s="22">
         <v>20</v>
       </c>
@@ -4417,7 +4555,7 @@
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
+      <c r="I21" s="54"/>
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
@@ -4426,10 +4564,14 @@
       <c r="O21" s="24"/>
       <c r="P21" s="24"/>
       <c r="Q21" s="24"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="17"/>
-    </row>
-    <row r="22" spans="1:19" thickBot="1">
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="17"/>
+    </row>
+    <row r="22" spans="1:23" thickBot="1">
       <c r="A22" s="22">
         <v>21</v>
       </c>
@@ -4440,7 +4582,7 @@
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
+      <c r="I22" s="54"/>
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
@@ -4449,10 +4591,14 @@
       <c r="O22" s="24"/>
       <c r="P22" s="24"/>
       <c r="Q22" s="24"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="17"/>
-    </row>
-    <row r="23" spans="1:19" thickBot="1">
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="25"/>
+      <c r="W22" s="17"/>
+    </row>
+    <row r="23" spans="1:23" thickBot="1">
       <c r="A23" s="22">
         <v>22</v>
       </c>
@@ -4463,7 +4609,7 @@
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
+      <c r="I23" s="54"/>
       <c r="J23" s="24"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
@@ -4472,10 +4618,14 @@
       <c r="O23" s="24"/>
       <c r="P23" s="24"/>
       <c r="Q23" s="24"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="17"/>
-    </row>
-    <row r="24" spans="1:19" thickBot="1">
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="17"/>
+    </row>
+    <row r="24" spans="1:23" thickBot="1">
       <c r="A24" s="22">
         <v>23</v>
       </c>
@@ -4486,7 +4636,7 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
+      <c r="I24" s="54"/>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
@@ -4495,10 +4645,14 @@
       <c r="O24" s="24"/>
       <c r="P24" s="24"/>
       <c r="Q24" s="24"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="17"/>
-    </row>
-    <row r="25" spans="1:19" thickBot="1">
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="17"/>
+    </row>
+    <row r="25" spans="1:23" thickBot="1">
       <c r="A25" s="22">
         <v>24</v>
       </c>
@@ -4509,7 +4663,7 @@
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
+      <c r="I25" s="54"/>
       <c r="J25" s="24"/>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
@@ -4518,10 +4672,14 @@
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
       <c r="Q25" s="24"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="17"/>
-    </row>
-    <row r="26" spans="1:19" thickBot="1">
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="17"/>
+    </row>
+    <row r="26" spans="1:23" thickBot="1">
       <c r="A26" s="22">
         <v>25</v>
       </c>
@@ -4532,7 +4690,7 @@
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="24"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
@@ -4541,10 +4699,14 @@
       <c r="O26" s="24"/>
       <c r="P26" s="24"/>
       <c r="Q26" s="24"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="17"/>
-    </row>
-    <row r="27" spans="1:19" thickBot="1">
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="17"/>
+    </row>
+    <row r="27" spans="1:23" thickBot="1">
       <c r="A27" s="22">
         <v>26</v>
       </c>
@@ -4555,7 +4717,7 @@
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="24"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
@@ -4564,10 +4726,14 @@
       <c r="O27" s="24"/>
       <c r="P27" s="24"/>
       <c r="Q27" s="24"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="17"/>
-    </row>
-    <row r="28" spans="1:19" thickBot="1">
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="24"/>
+      <c r="U27" s="24"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="17"/>
+    </row>
+    <row r="28" spans="1:23" thickBot="1">
       <c r="A28" s="22">
         <v>27</v>
       </c>
@@ -4578,7 +4744,7 @@
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
+      <c r="I28" s="54"/>
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
@@ -4587,10 +4753,14 @@
       <c r="O28" s="24"/>
       <c r="P28" s="24"/>
       <c r="Q28" s="24"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="17"/>
-    </row>
-    <row r="29" spans="1:19" thickBot="1">
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="25"/>
+      <c r="W28" s="17"/>
+    </row>
+    <row r="29" spans="1:23" thickBot="1">
       <c r="A29" s="22">
         <v>28</v>
       </c>
@@ -4601,7 +4771,7 @@
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
+      <c r="I29" s="54"/>
       <c r="J29" s="24"/>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
@@ -4610,10 +4780,14 @@
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
       <c r="Q29" s="24"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="17"/>
-    </row>
-    <row r="30" spans="1:19" thickBot="1">
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24"/>
+      <c r="U29" s="24"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="17"/>
+    </row>
+    <row r="30" spans="1:23" thickBot="1">
       <c r="A30" s="22">
         <v>29</v>
       </c>
@@ -4624,7 +4798,7 @@
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
+      <c r="I30" s="54"/>
       <c r="J30" s="24"/>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
@@ -4633,10 +4807,14 @@
       <c r="O30" s="24"/>
       <c r="P30" s="24"/>
       <c r="Q30" s="24"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="17"/>
-    </row>
-    <row r="31" spans="1:19" thickBot="1">
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="T30" s="24"/>
+      <c r="U30" s="24"/>
+      <c r="V30" s="25"/>
+      <c r="W30" s="17"/>
+    </row>
+    <row r="31" spans="1:23" thickBot="1">
       <c r="A31" s="22">
         <v>30</v>
       </c>
@@ -4647,7 +4825,7 @@
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
+      <c r="I31" s="54"/>
       <c r="J31" s="24"/>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
@@ -4656,10 +4834,14 @@
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
       <c r="Q31" s="24"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="17"/>
-    </row>
-    <row r="32" spans="1:19" thickBot="1">
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="25"/>
+      <c r="W31" s="17"/>
+    </row>
+    <row r="32" spans="1:23" thickBot="1">
       <c r="A32" s="22">
         <v>31</v>
       </c>
@@ -4670,7 +4852,7 @@
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
+      <c r="I32" s="54"/>
       <c r="J32" s="24"/>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
@@ -4679,10 +4861,14 @@
       <c r="O32" s="24"/>
       <c r="P32" s="24"/>
       <c r="Q32" s="24"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="17"/>
-    </row>
-    <row r="33" spans="1:19" thickBot="1">
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="24"/>
+      <c r="U32" s="24"/>
+      <c r="V32" s="25"/>
+      <c r="W32" s="17"/>
+    </row>
+    <row r="33" spans="1:23" thickBot="1">
       <c r="A33" s="22">
         <v>32</v>
       </c>
@@ -4693,7 +4879,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
+      <c r="I33" s="54"/>
       <c r="J33" s="24"/>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
@@ -4702,10 +4888,14 @@
       <c r="O33" s="24"/>
       <c r="P33" s="24"/>
       <c r="Q33" s="24"/>
-      <c r="R33" s="25"/>
-      <c r="S33" s="17"/>
-    </row>
-    <row r="34" spans="1:19" thickBot="1">
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="25"/>
+      <c r="W33" s="17"/>
+    </row>
+    <row r="34" spans="1:23" thickBot="1">
       <c r="A34" s="22">
         <v>33</v>
       </c>
@@ -4716,7 +4906,7 @@
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
+      <c r="I34" s="54"/>
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
@@ -4725,10 +4915,14 @@
       <c r="O34" s="24"/>
       <c r="P34" s="24"/>
       <c r="Q34" s="24"/>
-      <c r="R34" s="25"/>
-      <c r="S34" s="17"/>
-    </row>
-    <row r="35" spans="1:19" thickBot="1">
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="24"/>
+      <c r="U34" s="24"/>
+      <c r="V34" s="25"/>
+      <c r="W34" s="17"/>
+    </row>
+    <row r="35" spans="1:23" thickBot="1">
       <c r="A35" s="22">
         <v>34</v>
       </c>
@@ -4739,7 +4933,7 @@
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
+      <c r="I35" s="54"/>
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
@@ -4748,10 +4942,14 @@
       <c r="O35" s="24"/>
       <c r="P35" s="24"/>
       <c r="Q35" s="24"/>
-      <c r="R35" s="25"/>
-      <c r="S35" s="17"/>
-    </row>
-    <row r="36" spans="1:19" thickBot="1">
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="T35" s="24"/>
+      <c r="U35" s="24"/>
+      <c r="V35" s="25"/>
+      <c r="W35" s="17"/>
+    </row>
+    <row r="36" spans="1:23" thickBot="1">
       <c r="A36" s="22">
         <v>35</v>
       </c>
@@ -4762,7 +4960,7 @@
       <c r="F36" s="24"/>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
+      <c r="I36" s="54"/>
       <c r="J36" s="24"/>
       <c r="K36" s="24"/>
       <c r="L36" s="24"/>
@@ -4771,10 +4969,14 @@
       <c r="O36" s="24"/>
       <c r="P36" s="24"/>
       <c r="Q36" s="24"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="17"/>
-    </row>
-    <row r="37" spans="1:19" thickBot="1">
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="25"/>
+      <c r="W36" s="17"/>
+    </row>
+    <row r="37" spans="1:23" thickBot="1">
       <c r="A37" s="22">
         <v>36</v>
       </c>
@@ -4785,7 +4987,7 @@
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
       <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
+      <c r="I37" s="54"/>
       <c r="J37" s="24"/>
       <c r="K37" s="24"/>
       <c r="L37" s="24"/>
@@ -4794,10 +4996,14 @@
       <c r="O37" s="24"/>
       <c r="P37" s="24"/>
       <c r="Q37" s="24"/>
-      <c r="R37" s="25"/>
-      <c r="S37" s="17"/>
-    </row>
-    <row r="38" spans="1:19" thickBot="1">
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
+      <c r="U37" s="24"/>
+      <c r="V37" s="25"/>
+      <c r="W37" s="17"/>
+    </row>
+    <row r="38" spans="1:23" thickBot="1">
       <c r="A38" s="22">
         <v>37</v>
       </c>
@@ -4808,7 +5014,7 @@
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
+      <c r="I38" s="54"/>
       <c r="J38" s="24"/>
       <c r="K38" s="24"/>
       <c r="L38" s="24"/>
@@ -4817,10 +5023,14 @@
       <c r="O38" s="24"/>
       <c r="P38" s="24"/>
       <c r="Q38" s="24"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="17"/>
-    </row>
-    <row r="39" spans="1:19" thickBot="1">
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="24"/>
+      <c r="U38" s="24"/>
+      <c r="V38" s="25"/>
+      <c r="W38" s="17"/>
+    </row>
+    <row r="39" spans="1:23" thickBot="1">
       <c r="A39" s="22">
         <v>38</v>
       </c>
@@ -4831,7 +5041,7 @@
       <c r="F39" s="24"/>
       <c r="G39" s="24"/>
       <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
+      <c r="I39" s="54"/>
       <c r="J39" s="24"/>
       <c r="K39" s="24"/>
       <c r="L39" s="24"/>
@@ -4840,10 +5050,14 @@
       <c r="O39" s="24"/>
       <c r="P39" s="24"/>
       <c r="Q39" s="24"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="17"/>
-    </row>
-    <row r="40" spans="1:19" thickBot="1">
+      <c r="R39" s="24"/>
+      <c r="S39" s="24"/>
+      <c r="T39" s="24"/>
+      <c r="U39" s="24"/>
+      <c r="V39" s="25"/>
+      <c r="W39" s="17"/>
+    </row>
+    <row r="40" spans="1:23" thickBot="1">
       <c r="A40" s="22">
         <v>39</v>
       </c>
@@ -4854,7 +5068,7 @@
       <c r="F40" s="24"/>
       <c r="G40" s="24"/>
       <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
+      <c r="I40" s="54"/>
       <c r="J40" s="24"/>
       <c r="K40" s="24"/>
       <c r="L40" s="24"/>
@@ -4863,10 +5077,14 @@
       <c r="O40" s="24"/>
       <c r="P40" s="24"/>
       <c r="Q40" s="24"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="17"/>
-    </row>
-    <row r="41" spans="1:19" thickBot="1">
+      <c r="R40" s="24"/>
+      <c r="S40" s="24"/>
+      <c r="T40" s="24"/>
+      <c r="U40" s="24"/>
+      <c r="V40" s="25"/>
+      <c r="W40" s="17"/>
+    </row>
+    <row r="41" spans="1:23" thickBot="1">
       <c r="A41" s="22">
         <v>40</v>
       </c>
@@ -4877,7 +5095,7 @@
       <c r="F41" s="24"/>
       <c r="G41" s="24"/>
       <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
+      <c r="I41" s="54"/>
       <c r="J41" s="24"/>
       <c r="K41" s="24"/>
       <c r="L41" s="24"/>
@@ -4886,10 +5104,14 @@
       <c r="O41" s="24"/>
       <c r="P41" s="24"/>
       <c r="Q41" s="24"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="17"/>
-    </row>
-    <row r="42" spans="1:19" thickBot="1">
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="25"/>
+      <c r="W41" s="17"/>
+    </row>
+    <row r="42" spans="1:23" thickBot="1">
       <c r="A42" s="22">
         <v>41</v>
       </c>
@@ -4900,7 +5122,7 @@
       <c r="F42" s="24"/>
       <c r="G42" s="24"/>
       <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
+      <c r="I42" s="54"/>
       <c r="J42" s="24"/>
       <c r="K42" s="24"/>
       <c r="L42" s="24"/>
@@ -4909,10 +5131,14 @@
       <c r="O42" s="24"/>
       <c r="P42" s="24"/>
       <c r="Q42" s="24"/>
-      <c r="R42" s="25"/>
-      <c r="S42" s="17"/>
-    </row>
-    <row r="43" spans="1:19" thickBot="1">
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="25"/>
+      <c r="W42" s="17"/>
+    </row>
+    <row r="43" spans="1:23" thickBot="1">
       <c r="A43" s="22">
         <v>42</v>
       </c>
@@ -4923,7 +5149,7 @@
       <c r="F43" s="24"/>
       <c r="G43" s="24"/>
       <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
+      <c r="I43" s="54"/>
       <c r="J43" s="24"/>
       <c r="K43" s="24"/>
       <c r="L43" s="24"/>
@@ -4932,10 +5158,14 @@
       <c r="O43" s="24"/>
       <c r="P43" s="24"/>
       <c r="Q43" s="24"/>
-      <c r="R43" s="25"/>
-      <c r="S43" s="17"/>
-    </row>
-    <row r="44" spans="1:19" thickBot="1">
+      <c r="R43" s="24"/>
+      <c r="S43" s="24"/>
+      <c r="T43" s="24"/>
+      <c r="U43" s="24"/>
+      <c r="V43" s="25"/>
+      <c r="W43" s="17"/>
+    </row>
+    <row r="44" spans="1:23" thickBot="1">
       <c r="A44" s="22">
         <v>43</v>
       </c>
@@ -4946,7 +5176,7 @@
       <c r="F44" s="24"/>
       <c r="G44" s="24"/>
       <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
+      <c r="I44" s="54"/>
       <c r="J44" s="24"/>
       <c r="K44" s="24"/>
       <c r="L44" s="24"/>
@@ -4955,10 +5185,14 @@
       <c r="O44" s="24"/>
       <c r="P44" s="24"/>
       <c r="Q44" s="24"/>
-      <c r="R44" s="25"/>
-      <c r="S44" s="17"/>
-    </row>
-    <row r="45" spans="1:19" thickBot="1">
+      <c r="R44" s="24"/>
+      <c r="S44" s="24"/>
+      <c r="T44" s="24"/>
+      <c r="U44" s="24"/>
+      <c r="V44" s="25"/>
+      <c r="W44" s="17"/>
+    </row>
+    <row r="45" spans="1:23" thickBot="1">
       <c r="A45" s="22">
         <v>44</v>
       </c>
@@ -4969,7 +5203,7 @@
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
       <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
+      <c r="I45" s="54"/>
       <c r="J45" s="24"/>
       <c r="K45" s="24"/>
       <c r="L45" s="24"/>
@@ -4978,10 +5212,14 @@
       <c r="O45" s="24"/>
       <c r="P45" s="24"/>
       <c r="Q45" s="24"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="17"/>
-    </row>
-    <row r="46" spans="1:19" thickBot="1">
+      <c r="R45" s="24"/>
+      <c r="S45" s="24"/>
+      <c r="T45" s="24"/>
+      <c r="U45" s="24"/>
+      <c r="V45" s="25"/>
+      <c r="W45" s="17"/>
+    </row>
+    <row r="46" spans="1:23" thickBot="1">
       <c r="A46" s="22">
         <v>45</v>
       </c>
@@ -4992,7 +5230,7 @@
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
       <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
+      <c r="I46" s="54"/>
       <c r="J46" s="24"/>
       <c r="K46" s="24"/>
       <c r="L46" s="24"/>
@@ -5001,10 +5239,14 @@
       <c r="O46" s="24"/>
       <c r="P46" s="24"/>
       <c r="Q46" s="24"/>
-      <c r="R46" s="25"/>
-      <c r="S46" s="17"/>
-    </row>
-    <row r="47" spans="1:19" thickBot="1">
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="25"/>
+      <c r="W46" s="17"/>
+    </row>
+    <row r="47" spans="1:23" thickBot="1">
       <c r="A47" s="22">
         <v>46</v>
       </c>
@@ -5015,7 +5257,7 @@
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
       <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
+      <c r="I47" s="54"/>
       <c r="J47" s="24"/>
       <c r="K47" s="24"/>
       <c r="L47" s="24"/>
@@ -5024,10 +5266,14 @@
       <c r="O47" s="24"/>
       <c r="P47" s="24"/>
       <c r="Q47" s="24"/>
-      <c r="R47" s="25"/>
-      <c r="S47" s="17"/>
-    </row>
-    <row r="48" spans="1:19" thickBot="1">
+      <c r="R47" s="24"/>
+      <c r="S47" s="24"/>
+      <c r="T47" s="24"/>
+      <c r="U47" s="24"/>
+      <c r="V47" s="25"/>
+      <c r="W47" s="17"/>
+    </row>
+    <row r="48" spans="1:23" thickBot="1">
       <c r="A48" s="22">
         <v>47</v>
       </c>
@@ -5038,7 +5284,7 @@
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
       <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
+      <c r="I48" s="54"/>
       <c r="J48" s="24"/>
       <c r="K48" s="24"/>
       <c r="L48" s="24"/>
@@ -5047,10 +5293,14 @@
       <c r="O48" s="24"/>
       <c r="P48" s="24"/>
       <c r="Q48" s="24"/>
-      <c r="R48" s="25"/>
-      <c r="S48" s="17"/>
-    </row>
-    <row r="49" spans="1:19" thickBot="1">
+      <c r="R48" s="24"/>
+      <c r="S48" s="24"/>
+      <c r="T48" s="24"/>
+      <c r="U48" s="24"/>
+      <c r="V48" s="25"/>
+      <c r="W48" s="17"/>
+    </row>
+    <row r="49" spans="1:23" thickBot="1">
       <c r="A49" s="22">
         <v>48</v>
       </c>
@@ -5061,7 +5311,7 @@
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
+      <c r="I49" s="54"/>
       <c r="J49" s="24"/>
       <c r="K49" s="24"/>
       <c r="L49" s="24"/>
@@ -5070,10 +5320,14 @@
       <c r="O49" s="24"/>
       <c r="P49" s="24"/>
       <c r="Q49" s="24"/>
-      <c r="R49" s="25"/>
-      <c r="S49" s="17"/>
-    </row>
-    <row r="50" spans="1:19" thickBot="1">
+      <c r="R49" s="24"/>
+      <c r="S49" s="24"/>
+      <c r="T49" s="24"/>
+      <c r="U49" s="24"/>
+      <c r="V49" s="25"/>
+      <c r="W49" s="17"/>
+    </row>
+    <row r="50" spans="1:23" thickBot="1">
       <c r="A50" s="22">
         <v>49</v>
       </c>
@@ -5084,7 +5338,7 @@
       <c r="F50" s="24"/>
       <c r="G50" s="24"/>
       <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
+      <c r="I50" s="54"/>
       <c r="J50" s="24"/>
       <c r="K50" s="24"/>
       <c r="L50" s="24"/>
@@ -5093,10 +5347,14 @@
       <c r="O50" s="24"/>
       <c r="P50" s="24"/>
       <c r="Q50" s="24"/>
-      <c r="R50" s="25"/>
-      <c r="S50" s="17"/>
-    </row>
-    <row r="51" spans="1:19" thickBot="1">
+      <c r="R50" s="24"/>
+      <c r="S50" s="24"/>
+      <c r="T50" s="24"/>
+      <c r="U50" s="24"/>
+      <c r="V50" s="25"/>
+      <c r="W50" s="17"/>
+    </row>
+    <row r="51" spans="1:23" thickBot="1">
       <c r="A51" s="23">
         <v>50</v>
       </c>
@@ -5107,7 +5365,7 @@
       <c r="F51" s="26"/>
       <c r="G51" s="26"/>
       <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
+      <c r="I51" s="55"/>
       <c r="J51" s="26"/>
       <c r="K51" s="26"/>
       <c r="L51" s="26"/>
@@ -5116,10 +5374,14 @@
       <c r="O51" s="26"/>
       <c r="P51" s="26"/>
       <c r="Q51" s="26"/>
-      <c r="R51" s="27"/>
-      <c r="S51" s="17"/>
-    </row>
-    <row r="52" spans="1:19" ht="15" thickTop="1" thickBot="1">
+      <c r="R51" s="26"/>
+      <c r="S51" s="26"/>
+      <c r="T51" s="26"/>
+      <c r="U51" s="26"/>
+      <c r="V51" s="27"/>
+      <c r="W51" s="17"/>
+    </row>
+    <row r="52" spans="1:23" ht="15" thickTop="1" thickBot="1">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
@@ -5138,26 +5400,30 @@
       <c r="P52" s="18"/>
       <c r="Q52" s="18"/>
       <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="18"/>
+      <c r="U52" s="18"/>
+      <c r="V52" s="18"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="11">
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the volume of fuel in liters used during this trip (0-1000)." sqref="L2:L51">
+  <dataValidations count="16">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the volume of fuel in liters used during this trip (0-1000)." sqref="N2:N51">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must indicate whether a sail was used on this trip. Permitted values are:_x000d__x000d_Y : Yes_x000d_N: N" sqref="K2:K51">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must indicate whether a sail was used on this trip. Permitted values are:_x000d__x000d_Y : Yes_x000d_N: N" sqref="M2:M51">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total number of people onboard during thsi trip (1-20)." sqref="M2:M51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total number of people onboard during thsi trip (1-20)." sqref="O2:O51">
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total number of fish landed (0-10000). Leave blank if not known." sqref="Q2:Q51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total number of fish landed (0-10000). Leave blank if not known." sqref="U2:U51">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total value of the catch in Rupia (0-100000000). Leave blank if not known." sqref="R2:R51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total value of the catch in Rupia (0-100000000). Leave blank if not known." sqref="V2:V51">
       <formula1>0</formula1>
       <formula2>100000000</formula2>
     </dataValidation>
@@ -5172,17 +5438,34 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid time." sqref="I2:I51">
+    <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid time." sqref="J2:J51">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total weight of the catch in kilograms (0-10000). Leave blank if not known." sqref="P2:P51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total weight of the catch in kilograms (0-10000). Leave blank if not known." sqref="T2:T51">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid arrival time that is after the departure time." sqref="J2:J51">
-      <formula1>I2</formula1>
+    <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid arrival time that is after the departure time." sqref="K2:K51">
+      <formula1>J2</formula1>
       <formula2>0.999305555555556</formula2>
+    </dataValidation>
+    <dataValidation type="date" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid date" sqref="I2:I51">
+      <formula1>40909</formula1>
+      <formula2>55153</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="The following values are allowed:_x000d__x000d_OC - outrigger canoe" sqref="D2:D51">
+      <formula1>"OC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter 'Y' if the trip was aborted (e.g., due to poor weather or broken engine). Enter 'N' if the trip was not aborted." sqref="L2:L51">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the weight of ice in kg." sqref="Q2:Q51">
+      <formula1>0</formula1>
+      <formula2>99</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a recognized code for the sea conditions. Permitted values are:_x000d__x000d_1: Calm_x000d_2: Moderate_x000d_3: Rough" sqref="R2:R51">
+      <formula1>"1,2,3"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5200,13 +5483,13 @@
           <x14:formula1>
             <xm:f>'Gear Codes'!$A$2:$A$62</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N51</xm:sqref>
+          <xm:sqref>P2:P51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid fish ID code. Please check the &quot;Fish Codes&quot; tab.">
           <x14:formula1>
             <xm:f>'Species Codes'!A1:A1000</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O51</xm:sqref>
+          <xm:sqref>S2:S51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5222,7 +5505,7 @@
   <dimension ref="A1:F500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -5237,7 +5520,7 @@
         <v>45</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>32</v>
@@ -5246,7 +5529,7 @@
         <v>34</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="F1" s="7"/>
     </row>
@@ -9843,10 +10126,13 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E500">
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="Enter a whole number representing the length of the fish in mm." sqref="D2:D500">
       <formula1>1</formula1>
       <formula2>10000</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check you entry" error="Enter the sampling factor._x000d__x000d_Enter 'c' for conspicuous fish sampled from the entire catch._x000d__x000d_Enter 's' for sampled fish from the first basket unloaded." sqref="E2:E500">
+      <formula1>"c,s"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -9854,7 +10140,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="Please select a species code from the list. See the 'species codes' tab for a complete list. ">
           <x14:formula1>
             <xm:f>'Species Codes'!$A$2:$A$139</xm:f>
           </x14:formula1>
@@ -33580,7 +33866,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -33636,12 +33922,12 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="30" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="30" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -33671,17 +33957,18 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="30" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="30" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -33743,7 +34030,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -33754,97 +34041,97 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="38" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="B1" s="44"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="45" t="s">
-        <v>815</v>
+        <v>833</v>
       </c>
       <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="46" t="s">
-        <v>820</v>
+      <c r="A3" s="45" t="s">
+        <v>822</v>
       </c>
       <c r="B3" s="7"/>
     </row>
-    <row r="4" spans="1:2" ht="25">
-      <c r="A4" s="47" t="s">
-        <v>825</v>
+    <row r="4" spans="1:2">
+      <c r="A4" s="45" t="s">
+        <v>834</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="46" t="s">
-        <v>822</v>
+    <row r="5" spans="1:2" ht="25">
+      <c r="A5" s="48" t="s">
+        <v>823</v>
       </c>
       <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="45" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="45" t="s">
-        <v>812</v>
+      <c r="A7" s="46" t="s">
+        <v>816</v>
       </c>
       <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="46" t="s">
-        <v>821</v>
+      <c r="A8" s="45" t="s">
+        <v>819</v>
       </c>
       <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="46" t="s">
+        <v>832</v>
+      </c>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="46" t="s">
         <v>818</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="45" t="s">
-        <v>823</v>
-      </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="46" t="s">
-        <v>819</v>
+      <c r="A11" s="45" t="s">
+        <v>812</v>
       </c>
       <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="45" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:2" ht="25">
-      <c r="A13" s="48" t="s">
-        <v>827</v>
+    <row r="13" spans="1:2">
+      <c r="A13" s="46" t="s">
+        <v>835</v>
       </c>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="45" t="s">
-        <v>816</v>
+    <row r="14" spans="1:2" ht="25">
+      <c r="A14" s="47" t="s">
+        <v>821</v>
       </c>
       <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="45" t="s">
-        <v>826</v>
+      <c r="A15" s="46" t="s">
+        <v>817</v>
       </c>
       <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="45" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B16" s="7"/>
     </row>
@@ -33878,9 +34165,10 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState ref="A2:A16">
-    <sortCondition descending="1" ref="A2"/>
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
adds griddler route. fixes login text.
</commit_message>
<xml_diff>
--- a/public/Database.template.xlsx
+++ b/public/Database.template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="C470" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="10900" yWindow="660" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="560" windowWidth="25680" windowHeight="15500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -3951,7 +3951,7 @@
   <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" thickBottom="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updates database spreadsheet. updates province show view
</commit_message>
<xml_diff>
--- a/public/Database.template.xlsx
+++ b/public/Database.template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="846">
   <si>
     <t>Form A</t>
   </si>
@@ -2566,9 +2566,6 @@
   </si>
   <si>
     <t>Wave</t>
-  </si>
-  <si>
-    <t>Arr. Date</t>
   </si>
 </sst>
 </file>
@@ -3973,7 +3970,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X52"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -3984,11 +3981,10 @@
     <col min="1" max="1" width="4" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="10.83203125" style="16"/>
     <col min="10" max="10" width="15.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="16"/>
+    <col min="11" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" thickTop="1" thickBot="1">
+    <row r="1" spans="1:23" ht="15" thickTop="1" thickBot="1">
       <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
@@ -4020,47 +4016,44 @@
         <v>13</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>846</v>
+        <v>15</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>15</v>
+        <v>834</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>834</v>
+        <v>17</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="20" t="s">
-        <v>23</v>
+        <v>833</v>
       </c>
       <c r="R1" s="20" t="s">
-        <v>833</v>
+        <v>845</v>
       </c>
       <c r="S1" s="20" t="s">
-        <v>845</v>
+        <v>805</v>
       </c>
       <c r="T1" s="20" t="s">
-        <v>805</v>
+        <v>25</v>
       </c>
       <c r="U1" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="17"/>
-    </row>
-    <row r="2" spans="1:24" thickBot="1">
+      <c r="W1" s="17"/>
+    </row>
+    <row r="2" spans="1:23" thickBot="1">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -4073,9 +4066,9 @@
       <c r="H2" s="24"/>
       <c r="I2" s="54"/>
       <c r="J2" s="49"/>
-      <c r="K2" s="54"/>
+      <c r="K2" s="49"/>
       <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="M2" s="24"/>
       <c r="N2" s="24"/>
       <c r="O2" s="24"/>
       <c r="P2" s="24"/>
@@ -4084,11 +4077,10 @@
       <c r="S2" s="24"/>
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="17"/>
-    </row>
-    <row r="3" spans="1:24" thickBot="1">
+      <c r="V2" s="25"/>
+      <c r="W2" s="17"/>
+    </row>
+    <row r="3" spans="1:23" thickBot="1">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -4101,9 +4093,9 @@
       <c r="H3" s="24"/>
       <c r="I3" s="54"/>
       <c r="J3" s="49"/>
-      <c r="K3" s="54"/>
+      <c r="K3" s="49"/>
       <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
+      <c r="M3" s="24"/>
       <c r="N3" s="24"/>
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
@@ -4112,11 +4104,10 @@
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
       <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="17"/>
-    </row>
-    <row r="4" spans="1:24" thickBot="1">
+      <c r="V3" s="25"/>
+      <c r="W3" s="17"/>
+    </row>
+    <row r="4" spans="1:23" thickBot="1">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -4129,9 +4120,9 @@
       <c r="H4" s="24"/>
       <c r="I4" s="54"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="54"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
+      <c r="M4" s="24"/>
       <c r="N4" s="24"/>
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
@@ -4140,11 +4131,10 @@
       <c r="S4" s="24"/>
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="17"/>
-    </row>
-    <row r="5" spans="1:24" thickBot="1">
+      <c r="V4" s="25"/>
+      <c r="W4" s="17"/>
+    </row>
+    <row r="5" spans="1:23" thickBot="1">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -4157,7 +4147,7 @@
       <c r="H5" s="24"/>
       <c r="I5" s="54"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="54"/>
+      <c r="K5" s="24"/>
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
       <c r="N5" s="24"/>
@@ -4168,11 +4158,10 @@
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="17"/>
-    </row>
-    <row r="6" spans="1:24" thickBot="1">
+      <c r="V5" s="25"/>
+      <c r="W5" s="17"/>
+    </row>
+    <row r="6" spans="1:23" thickBot="1">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -4185,7 +4174,7 @@
       <c r="H6" s="24"/>
       <c r="I6" s="54"/>
       <c r="J6" s="24"/>
-      <c r="K6" s="54"/>
+      <c r="K6" s="24"/>
       <c r="L6" s="24"/>
       <c r="M6" s="24"/>
       <c r="N6" s="24"/>
@@ -4196,11 +4185,10 @@
       <c r="S6" s="24"/>
       <c r="T6" s="24"/>
       <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="17"/>
-    </row>
-    <row r="7" spans="1:24" thickBot="1">
+      <c r="V6" s="25"/>
+      <c r="W6" s="17"/>
+    </row>
+    <row r="7" spans="1:23" thickBot="1">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -4213,7 +4201,7 @@
       <c r="H7" s="24"/>
       <c r="I7" s="54"/>
       <c r="J7" s="24"/>
-      <c r="K7" s="54"/>
+      <c r="K7" s="24"/>
       <c r="L7" s="24"/>
       <c r="M7" s="24"/>
       <c r="N7" s="24"/>
@@ -4224,11 +4212,10 @@
       <c r="S7" s="24"/>
       <c r="T7" s="24"/>
       <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="17"/>
-    </row>
-    <row r="8" spans="1:24" thickBot="1">
+      <c r="V7" s="25"/>
+      <c r="W7" s="17"/>
+    </row>
+    <row r="8" spans="1:23" thickBot="1">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -4241,7 +4228,7 @@
       <c r="H8" s="24"/>
       <c r="I8" s="54"/>
       <c r="J8" s="24"/>
-      <c r="K8" s="54"/>
+      <c r="K8" s="24"/>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
       <c r="N8" s="24"/>
@@ -4252,11 +4239,10 @@
       <c r="S8" s="24"/>
       <c r="T8" s="24"/>
       <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="17"/>
-    </row>
-    <row r="9" spans="1:24" thickBot="1">
+      <c r="V8" s="25"/>
+      <c r="W8" s="17"/>
+    </row>
+    <row r="9" spans="1:23" thickBot="1">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -4269,7 +4255,7 @@
       <c r="H9" s="24"/>
       <c r="I9" s="54"/>
       <c r="J9" s="24"/>
-      <c r="K9" s="54"/>
+      <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
@@ -4280,11 +4266,10 @@
       <c r="S9" s="24"/>
       <c r="T9" s="24"/>
       <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="17"/>
-    </row>
-    <row r="10" spans="1:24" thickBot="1">
+      <c r="V9" s="25"/>
+      <c r="W9" s="17"/>
+    </row>
+    <row r="10" spans="1:23" thickBot="1">
       <c r="A10" s="22">
         <v>9</v>
       </c>
@@ -4297,7 +4282,7 @@
       <c r="H10" s="24"/>
       <c r="I10" s="54"/>
       <c r="J10" s="24"/>
-      <c r="K10" s="54"/>
+      <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
       <c r="N10" s="24"/>
@@ -4308,11 +4293,10 @@
       <c r="S10" s="24"/>
       <c r="T10" s="24"/>
       <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="17"/>
-    </row>
-    <row r="11" spans="1:24" thickBot="1">
+      <c r="V10" s="25"/>
+      <c r="W10" s="17"/>
+    </row>
+    <row r="11" spans="1:23" thickBot="1">
       <c r="A11" s="22">
         <v>10</v>
       </c>
@@ -4325,7 +4309,7 @@
       <c r="H11" s="24"/>
       <c r="I11" s="54"/>
       <c r="J11" s="24"/>
-      <c r="K11" s="54"/>
+      <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
       <c r="N11" s="24"/>
@@ -4336,11 +4320,10 @@
       <c r="S11" s="24"/>
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="17"/>
-    </row>
-    <row r="12" spans="1:24" thickBot="1">
+      <c r="V11" s="25"/>
+      <c r="W11" s="17"/>
+    </row>
+    <row r="12" spans="1:23" thickBot="1">
       <c r="A12" s="22">
         <v>11</v>
       </c>
@@ -4353,7 +4336,7 @@
       <c r="H12" s="24"/>
       <c r="I12" s="54"/>
       <c r="J12" s="24"/>
-      <c r="K12" s="54"/>
+      <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
@@ -4364,11 +4347,10 @@
       <c r="S12" s="24"/>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="17"/>
-    </row>
-    <row r="13" spans="1:24" thickBot="1">
+      <c r="V12" s="25"/>
+      <c r="W12" s="17"/>
+    </row>
+    <row r="13" spans="1:23" thickBot="1">
       <c r="A13" s="22">
         <v>12</v>
       </c>
@@ -4381,7 +4363,7 @@
       <c r="H13" s="24"/>
       <c r="I13" s="54"/>
       <c r="J13" s="24"/>
-      <c r="K13" s="54"/>
+      <c r="K13" s="24"/>
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
@@ -4392,11 +4374,10 @@
       <c r="S13" s="24"/>
       <c r="T13" s="24"/>
       <c r="U13" s="24"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="17"/>
-    </row>
-    <row r="14" spans="1:24" thickBot="1">
+      <c r="V13" s="25"/>
+      <c r="W13" s="17"/>
+    </row>
+    <row r="14" spans="1:23" thickBot="1">
       <c r="A14" s="22">
         <v>13</v>
       </c>
@@ -4409,7 +4390,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="54"/>
       <c r="J14" s="24"/>
-      <c r="K14" s="54"/>
+      <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
@@ -4420,11 +4401,10 @@
       <c r="S14" s="24"/>
       <c r="T14" s="24"/>
       <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="17"/>
-    </row>
-    <row r="15" spans="1:24" thickBot="1">
+      <c r="V14" s="25"/>
+      <c r="W14" s="17"/>
+    </row>
+    <row r="15" spans="1:23" thickBot="1">
       <c r="A15" s="22">
         <v>14</v>
       </c>
@@ -4437,7 +4417,7 @@
       <c r="H15" s="24"/>
       <c r="I15" s="54"/>
       <c r="J15" s="24"/>
-      <c r="K15" s="54"/>
+      <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
@@ -4448,11 +4428,10 @@
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
       <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="17"/>
-    </row>
-    <row r="16" spans="1:24" thickBot="1">
+      <c r="V15" s="25"/>
+      <c r="W15" s="17"/>
+    </row>
+    <row r="16" spans="1:23" thickBot="1">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -4465,7 +4444,7 @@
       <c r="H16" s="24"/>
       <c r="I16" s="54"/>
       <c r="J16" s="24"/>
-      <c r="K16" s="54"/>
+      <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
       <c r="N16" s="24"/>
@@ -4476,11 +4455,10 @@
       <c r="S16" s="24"/>
       <c r="T16" s="24"/>
       <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="17"/>
-    </row>
-    <row r="17" spans="1:24" thickBot="1">
+      <c r="V16" s="25"/>
+      <c r="W16" s="17"/>
+    </row>
+    <row r="17" spans="1:23" thickBot="1">
       <c r="A17" s="22">
         <v>16</v>
       </c>
@@ -4493,7 +4471,7 @@
       <c r="H17" s="24"/>
       <c r="I17" s="54"/>
       <c r="J17" s="24"/>
-      <c r="K17" s="54"/>
+      <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
       <c r="N17" s="24"/>
@@ -4504,11 +4482,10 @@
       <c r="S17" s="24"/>
       <c r="T17" s="24"/>
       <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="17"/>
-    </row>
-    <row r="18" spans="1:24" thickBot="1">
+      <c r="V17" s="25"/>
+      <c r="W17" s="17"/>
+    </row>
+    <row r="18" spans="1:23" thickBot="1">
       <c r="A18" s="22">
         <v>17</v>
       </c>
@@ -4521,7 +4498,7 @@
       <c r="H18" s="24"/>
       <c r="I18" s="54"/>
       <c r="J18" s="24"/>
-      <c r="K18" s="54"/>
+      <c r="K18" s="24"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
       <c r="N18" s="24"/>
@@ -4532,11 +4509,10 @@
       <c r="S18" s="24"/>
       <c r="T18" s="24"/>
       <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="25"/>
-      <c r="X18" s="17"/>
-    </row>
-    <row r="19" spans="1:24" thickBot="1">
+      <c r="V18" s="25"/>
+      <c r="W18" s="17"/>
+    </row>
+    <row r="19" spans="1:23" thickBot="1">
       <c r="A19" s="22">
         <v>18</v>
       </c>
@@ -4549,7 +4525,7 @@
       <c r="H19" s="24"/>
       <c r="I19" s="54"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="54"/>
+      <c r="K19" s="24"/>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
@@ -4560,11 +4536,10 @@
       <c r="S19" s="24"/>
       <c r="T19" s="24"/>
       <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="25"/>
-      <c r="X19" s="17"/>
-    </row>
-    <row r="20" spans="1:24" thickBot="1">
+      <c r="V19" s="25"/>
+      <c r="W19" s="17"/>
+    </row>
+    <row r="20" spans="1:23" thickBot="1">
       <c r="A20" s="22">
         <v>19</v>
       </c>
@@ -4577,7 +4552,7 @@
       <c r="H20" s="24"/>
       <c r="I20" s="54"/>
       <c r="J20" s="24"/>
-      <c r="K20" s="54"/>
+      <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
@@ -4588,11 +4563,10 @@
       <c r="S20" s="24"/>
       <c r="T20" s="24"/>
       <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="25"/>
-      <c r="X20" s="17"/>
-    </row>
-    <row r="21" spans="1:24" thickBot="1">
+      <c r="V20" s="25"/>
+      <c r="W20" s="17"/>
+    </row>
+    <row r="21" spans="1:23" thickBot="1">
       <c r="A21" s="22">
         <v>20</v>
       </c>
@@ -4605,7 +4579,7 @@
       <c r="H21" s="24"/>
       <c r="I21" s="54"/>
       <c r="J21" s="24"/>
-      <c r="K21" s="54"/>
+      <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
@@ -4616,11 +4590,10 @@
       <c r="S21" s="24"/>
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="25"/>
-      <c r="X21" s="17"/>
-    </row>
-    <row r="22" spans="1:24" thickBot="1">
+      <c r="V21" s="25"/>
+      <c r="W21" s="17"/>
+    </row>
+    <row r="22" spans="1:23" thickBot="1">
       <c r="A22" s="22">
         <v>21</v>
       </c>
@@ -4633,7 +4606,7 @@
       <c r="H22" s="24"/>
       <c r="I22" s="54"/>
       <c r="J22" s="24"/>
-      <c r="K22" s="54"/>
+      <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
@@ -4644,11 +4617,10 @@
       <c r="S22" s="24"/>
       <c r="T22" s="24"/>
       <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="25"/>
-      <c r="X22" s="17"/>
-    </row>
-    <row r="23" spans="1:24" thickBot="1">
+      <c r="V22" s="25"/>
+      <c r="W22" s="17"/>
+    </row>
+    <row r="23" spans="1:23" thickBot="1">
       <c r="A23" s="22">
         <v>22</v>
       </c>
@@ -4661,7 +4633,7 @@
       <c r="H23" s="24"/>
       <c r="I23" s="54"/>
       <c r="J23" s="24"/>
-      <c r="K23" s="54"/>
+      <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
@@ -4672,11 +4644,10 @@
       <c r="S23" s="24"/>
       <c r="T23" s="24"/>
       <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="25"/>
-      <c r="X23" s="17"/>
-    </row>
-    <row r="24" spans="1:24" thickBot="1">
+      <c r="V23" s="25"/>
+      <c r="W23" s="17"/>
+    </row>
+    <row r="24" spans="1:23" thickBot="1">
       <c r="A24" s="22">
         <v>23</v>
       </c>
@@ -4689,7 +4660,7 @@
       <c r="H24" s="24"/>
       <c r="I24" s="54"/>
       <c r="J24" s="24"/>
-      <c r="K24" s="54"/>
+      <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
@@ -4700,11 +4671,10 @@
       <c r="S24" s="24"/>
       <c r="T24" s="24"/>
       <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="25"/>
-      <c r="X24" s="17"/>
-    </row>
-    <row r="25" spans="1:24" thickBot="1">
+      <c r="V24" s="25"/>
+      <c r="W24" s="17"/>
+    </row>
+    <row r="25" spans="1:23" thickBot="1">
       <c r="A25" s="22">
         <v>24</v>
       </c>
@@ -4717,7 +4687,7 @@
       <c r="H25" s="24"/>
       <c r="I25" s="54"/>
       <c r="J25" s="24"/>
-      <c r="K25" s="54"/>
+      <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
@@ -4728,11 +4698,10 @@
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
       <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="25"/>
-      <c r="X25" s="17"/>
-    </row>
-    <row r="26" spans="1:24" thickBot="1">
+      <c r="V25" s="25"/>
+      <c r="W25" s="17"/>
+    </row>
+    <row r="26" spans="1:23" thickBot="1">
       <c r="A26" s="22">
         <v>25</v>
       </c>
@@ -4745,7 +4714,7 @@
       <c r="H26" s="24"/>
       <c r="I26" s="54"/>
       <c r="J26" s="24"/>
-      <c r="K26" s="54"/>
+      <c r="K26" s="24"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
@@ -4756,11 +4725,10 @@
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
       <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="25"/>
-      <c r="X26" s="17"/>
-    </row>
-    <row r="27" spans="1:24" thickBot="1">
+      <c r="V26" s="25"/>
+      <c r="W26" s="17"/>
+    </row>
+    <row r="27" spans="1:23" thickBot="1">
       <c r="A27" s="22">
         <v>26</v>
       </c>
@@ -4773,7 +4741,7 @@
       <c r="H27" s="24"/>
       <c r="I27" s="54"/>
       <c r="J27" s="24"/>
-      <c r="K27" s="54"/>
+      <c r="K27" s="24"/>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
       <c r="N27" s="24"/>
@@ -4784,11 +4752,10 @@
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
       <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="25"/>
-      <c r="X27" s="17"/>
-    </row>
-    <row r="28" spans="1:24" thickBot="1">
+      <c r="V27" s="25"/>
+      <c r="W27" s="17"/>
+    </row>
+    <row r="28" spans="1:23" thickBot="1">
       <c r="A28" s="22">
         <v>27</v>
       </c>
@@ -4801,7 +4768,7 @@
       <c r="H28" s="24"/>
       <c r="I28" s="54"/>
       <c r="J28" s="24"/>
-      <c r="K28" s="54"/>
+      <c r="K28" s="24"/>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
       <c r="N28" s="24"/>
@@ -4812,11 +4779,10 @@
       <c r="S28" s="24"/>
       <c r="T28" s="24"/>
       <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="25"/>
-      <c r="X28" s="17"/>
-    </row>
-    <row r="29" spans="1:24" thickBot="1">
+      <c r="V28" s="25"/>
+      <c r="W28" s="17"/>
+    </row>
+    <row r="29" spans="1:23" thickBot="1">
       <c r="A29" s="22">
         <v>28</v>
       </c>
@@ -4829,7 +4795,7 @@
       <c r="H29" s="24"/>
       <c r="I29" s="54"/>
       <c r="J29" s="24"/>
-      <c r="K29" s="54"/>
+      <c r="K29" s="24"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
@@ -4840,11 +4806,10 @@
       <c r="S29" s="24"/>
       <c r="T29" s="24"/>
       <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="25"/>
-      <c r="X29" s="17"/>
-    </row>
-    <row r="30" spans="1:24" thickBot="1">
+      <c r="V29" s="25"/>
+      <c r="W29" s="17"/>
+    </row>
+    <row r="30" spans="1:23" thickBot="1">
       <c r="A30" s="22">
         <v>29</v>
       </c>
@@ -4857,7 +4822,7 @@
       <c r="H30" s="24"/>
       <c r="I30" s="54"/>
       <c r="J30" s="24"/>
-      <c r="K30" s="54"/>
+      <c r="K30" s="24"/>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
       <c r="N30" s="24"/>
@@ -4868,11 +4833,10 @@
       <c r="S30" s="24"/>
       <c r="T30" s="24"/>
       <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="25"/>
-      <c r="X30" s="17"/>
-    </row>
-    <row r="31" spans="1:24" thickBot="1">
+      <c r="V30" s="25"/>
+      <c r="W30" s="17"/>
+    </row>
+    <row r="31" spans="1:23" thickBot="1">
       <c r="A31" s="22">
         <v>30</v>
       </c>
@@ -4885,7 +4849,7 @@
       <c r="H31" s="24"/>
       <c r="I31" s="54"/>
       <c r="J31" s="24"/>
-      <c r="K31" s="54"/>
+      <c r="K31" s="24"/>
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
@@ -4896,11 +4860,10 @@
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
       <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="25"/>
-      <c r="X31" s="17"/>
-    </row>
-    <row r="32" spans="1:24" thickBot="1">
+      <c r="V31" s="25"/>
+      <c r="W31" s="17"/>
+    </row>
+    <row r="32" spans="1:23" thickBot="1">
       <c r="A32" s="22">
         <v>31</v>
       </c>
@@ -4913,7 +4876,7 @@
       <c r="H32" s="24"/>
       <c r="I32" s="54"/>
       <c r="J32" s="24"/>
-      <c r="K32" s="54"/>
+      <c r="K32" s="24"/>
       <c r="L32" s="24"/>
       <c r="M32" s="24"/>
       <c r="N32" s="24"/>
@@ -4924,11 +4887,10 @@
       <c r="S32" s="24"/>
       <c r="T32" s="24"/>
       <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="25"/>
-      <c r="X32" s="17"/>
-    </row>
-    <row r="33" spans="1:24" thickBot="1">
+      <c r="V32" s="25"/>
+      <c r="W32" s="17"/>
+    </row>
+    <row r="33" spans="1:23" thickBot="1">
       <c r="A33" s="22">
         <v>32</v>
       </c>
@@ -4941,7 +4903,7 @@
       <c r="H33" s="24"/>
       <c r="I33" s="54"/>
       <c r="J33" s="24"/>
-      <c r="K33" s="54"/>
+      <c r="K33" s="24"/>
       <c r="L33" s="24"/>
       <c r="M33" s="24"/>
       <c r="N33" s="24"/>
@@ -4952,11 +4914,10 @@
       <c r="S33" s="24"/>
       <c r="T33" s="24"/>
       <c r="U33" s="24"/>
-      <c r="V33" s="24"/>
-      <c r="W33" s="25"/>
-      <c r="X33" s="17"/>
-    </row>
-    <row r="34" spans="1:24" thickBot="1">
+      <c r="V33" s="25"/>
+      <c r="W33" s="17"/>
+    </row>
+    <row r="34" spans="1:23" thickBot="1">
       <c r="A34" s="22">
         <v>33</v>
       </c>
@@ -4969,7 +4930,7 @@
       <c r="H34" s="24"/>
       <c r="I34" s="54"/>
       <c r="J34" s="24"/>
-      <c r="K34" s="54"/>
+      <c r="K34" s="24"/>
       <c r="L34" s="24"/>
       <c r="M34" s="24"/>
       <c r="N34" s="24"/>
@@ -4980,11 +4941,10 @@
       <c r="S34" s="24"/>
       <c r="T34" s="24"/>
       <c r="U34" s="24"/>
-      <c r="V34" s="24"/>
-      <c r="W34" s="25"/>
-      <c r="X34" s="17"/>
-    </row>
-    <row r="35" spans="1:24" thickBot="1">
+      <c r="V34" s="25"/>
+      <c r="W34" s="17"/>
+    </row>
+    <row r="35" spans="1:23" thickBot="1">
       <c r="A35" s="22">
         <v>34</v>
       </c>
@@ -4997,7 +4957,7 @@
       <c r="H35" s="24"/>
       <c r="I35" s="54"/>
       <c r="J35" s="24"/>
-      <c r="K35" s="54"/>
+      <c r="K35" s="24"/>
       <c r="L35" s="24"/>
       <c r="M35" s="24"/>
       <c r="N35" s="24"/>
@@ -5008,11 +4968,10 @@
       <c r="S35" s="24"/>
       <c r="T35" s="24"/>
       <c r="U35" s="24"/>
-      <c r="V35" s="24"/>
-      <c r="W35" s="25"/>
-      <c r="X35" s="17"/>
-    </row>
-    <row r="36" spans="1:24" thickBot="1">
+      <c r="V35" s="25"/>
+      <c r="W35" s="17"/>
+    </row>
+    <row r="36" spans="1:23" thickBot="1">
       <c r="A36" s="22">
         <v>35</v>
       </c>
@@ -5025,7 +4984,7 @@
       <c r="H36" s="24"/>
       <c r="I36" s="54"/>
       <c r="J36" s="24"/>
-      <c r="K36" s="54"/>
+      <c r="K36" s="24"/>
       <c r="L36" s="24"/>
       <c r="M36" s="24"/>
       <c r="N36" s="24"/>
@@ -5036,11 +4995,10 @@
       <c r="S36" s="24"/>
       <c r="T36" s="24"/>
       <c r="U36" s="24"/>
-      <c r="V36" s="24"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="17"/>
-    </row>
-    <row r="37" spans="1:24" thickBot="1">
+      <c r="V36" s="25"/>
+      <c r="W36" s="17"/>
+    </row>
+    <row r="37" spans="1:23" thickBot="1">
       <c r="A37" s="22">
         <v>36</v>
       </c>
@@ -5053,7 +5011,7 @@
       <c r="H37" s="24"/>
       <c r="I37" s="54"/>
       <c r="J37" s="24"/>
-      <c r="K37" s="54"/>
+      <c r="K37" s="24"/>
       <c r="L37" s="24"/>
       <c r="M37" s="24"/>
       <c r="N37" s="24"/>
@@ -5064,11 +5022,10 @@
       <c r="S37" s="24"/>
       <c r="T37" s="24"/>
       <c r="U37" s="24"/>
-      <c r="V37" s="24"/>
-      <c r="W37" s="25"/>
-      <c r="X37" s="17"/>
-    </row>
-    <row r="38" spans="1:24" thickBot="1">
+      <c r="V37" s="25"/>
+      <c r="W37" s="17"/>
+    </row>
+    <row r="38" spans="1:23" thickBot="1">
       <c r="A38" s="22">
         <v>37</v>
       </c>
@@ -5081,7 +5038,7 @@
       <c r="H38" s="24"/>
       <c r="I38" s="54"/>
       <c r="J38" s="24"/>
-      <c r="K38" s="54"/>
+      <c r="K38" s="24"/>
       <c r="L38" s="24"/>
       <c r="M38" s="24"/>
       <c r="N38" s="24"/>
@@ -5092,11 +5049,10 @@
       <c r="S38" s="24"/>
       <c r="T38" s="24"/>
       <c r="U38" s="24"/>
-      <c r="V38" s="24"/>
-      <c r="W38" s="25"/>
-      <c r="X38" s="17"/>
-    </row>
-    <row r="39" spans="1:24" thickBot="1">
+      <c r="V38" s="25"/>
+      <c r="W38" s="17"/>
+    </row>
+    <row r="39" spans="1:23" thickBot="1">
       <c r="A39" s="22">
         <v>38</v>
       </c>
@@ -5109,7 +5065,7 @@
       <c r="H39" s="24"/>
       <c r="I39" s="54"/>
       <c r="J39" s="24"/>
-      <c r="K39" s="54"/>
+      <c r="K39" s="24"/>
       <c r="L39" s="24"/>
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
@@ -5120,11 +5076,10 @@
       <c r="S39" s="24"/>
       <c r="T39" s="24"/>
       <c r="U39" s="24"/>
-      <c r="V39" s="24"/>
-      <c r="W39" s="25"/>
-      <c r="X39" s="17"/>
-    </row>
-    <row r="40" spans="1:24" thickBot="1">
+      <c r="V39" s="25"/>
+      <c r="W39" s="17"/>
+    </row>
+    <row r="40" spans="1:23" thickBot="1">
       <c r="A40" s="22">
         <v>39</v>
       </c>
@@ -5137,7 +5092,7 @@
       <c r="H40" s="24"/>
       <c r="I40" s="54"/>
       <c r="J40" s="24"/>
-      <c r="K40" s="54"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="24"/>
       <c r="M40" s="24"/>
       <c r="N40" s="24"/>
@@ -5148,11 +5103,10 @@
       <c r="S40" s="24"/>
       <c r="T40" s="24"/>
       <c r="U40" s="24"/>
-      <c r="V40" s="24"/>
-      <c r="W40" s="25"/>
-      <c r="X40" s="17"/>
-    </row>
-    <row r="41" spans="1:24" thickBot="1">
+      <c r="V40" s="25"/>
+      <c r="W40" s="17"/>
+    </row>
+    <row r="41" spans="1:23" thickBot="1">
       <c r="A41" s="22">
         <v>40</v>
       </c>
@@ -5165,7 +5119,7 @@
       <c r="H41" s="24"/>
       <c r="I41" s="54"/>
       <c r="J41" s="24"/>
-      <c r="K41" s="54"/>
+      <c r="K41" s="24"/>
       <c r="L41" s="24"/>
       <c r="M41" s="24"/>
       <c r="N41" s="24"/>
@@ -5176,11 +5130,10 @@
       <c r="S41" s="24"/>
       <c r="T41" s="24"/>
       <c r="U41" s="24"/>
-      <c r="V41" s="24"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="17"/>
-    </row>
-    <row r="42" spans="1:24" thickBot="1">
+      <c r="V41" s="25"/>
+      <c r="W41" s="17"/>
+    </row>
+    <row r="42" spans="1:23" thickBot="1">
       <c r="A42" s="22">
         <v>41</v>
       </c>
@@ -5193,7 +5146,7 @@
       <c r="H42" s="24"/>
       <c r="I42" s="54"/>
       <c r="J42" s="24"/>
-      <c r="K42" s="54"/>
+      <c r="K42" s="24"/>
       <c r="L42" s="24"/>
       <c r="M42" s="24"/>
       <c r="N42" s="24"/>
@@ -5204,11 +5157,10 @@
       <c r="S42" s="24"/>
       <c r="T42" s="24"/>
       <c r="U42" s="24"/>
-      <c r="V42" s="24"/>
-      <c r="W42" s="25"/>
-      <c r="X42" s="17"/>
-    </row>
-    <row r="43" spans="1:24" thickBot="1">
+      <c r="V42" s="25"/>
+      <c r="W42" s="17"/>
+    </row>
+    <row r="43" spans="1:23" thickBot="1">
       <c r="A43" s="22">
         <v>42</v>
       </c>
@@ -5221,7 +5173,7 @@
       <c r="H43" s="24"/>
       <c r="I43" s="54"/>
       <c r="J43" s="24"/>
-      <c r="K43" s="54"/>
+      <c r="K43" s="24"/>
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
       <c r="N43" s="24"/>
@@ -5232,11 +5184,10 @@
       <c r="S43" s="24"/>
       <c r="T43" s="24"/>
       <c r="U43" s="24"/>
-      <c r="V43" s="24"/>
-      <c r="W43" s="25"/>
-      <c r="X43" s="17"/>
-    </row>
-    <row r="44" spans="1:24" thickBot="1">
+      <c r="V43" s="25"/>
+      <c r="W43" s="17"/>
+    </row>
+    <row r="44" spans="1:23" thickBot="1">
       <c r="A44" s="22">
         <v>43</v>
       </c>
@@ -5249,7 +5200,7 @@
       <c r="H44" s="24"/>
       <c r="I44" s="54"/>
       <c r="J44" s="24"/>
-      <c r="K44" s="54"/>
+      <c r="K44" s="24"/>
       <c r="L44" s="24"/>
       <c r="M44" s="24"/>
       <c r="N44" s="24"/>
@@ -5260,11 +5211,10 @@
       <c r="S44" s="24"/>
       <c r="T44" s="24"/>
       <c r="U44" s="24"/>
-      <c r="V44" s="24"/>
-      <c r="W44" s="25"/>
-      <c r="X44" s="17"/>
-    </row>
-    <row r="45" spans="1:24" thickBot="1">
+      <c r="V44" s="25"/>
+      <c r="W44" s="17"/>
+    </row>
+    <row r="45" spans="1:23" thickBot="1">
       <c r="A45" s="22">
         <v>44</v>
       </c>
@@ -5277,7 +5227,7 @@
       <c r="H45" s="24"/>
       <c r="I45" s="54"/>
       <c r="J45" s="24"/>
-      <c r="K45" s="54"/>
+      <c r="K45" s="24"/>
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
       <c r="N45" s="24"/>
@@ -5288,11 +5238,10 @@
       <c r="S45" s="24"/>
       <c r="T45" s="24"/>
       <c r="U45" s="24"/>
-      <c r="V45" s="24"/>
-      <c r="W45" s="25"/>
-      <c r="X45" s="17"/>
-    </row>
-    <row r="46" spans="1:24" thickBot="1">
+      <c r="V45" s="25"/>
+      <c r="W45" s="17"/>
+    </row>
+    <row r="46" spans="1:23" thickBot="1">
       <c r="A46" s="22">
         <v>45</v>
       </c>
@@ -5305,7 +5254,7 @@
       <c r="H46" s="24"/>
       <c r="I46" s="54"/>
       <c r="J46" s="24"/>
-      <c r="K46" s="54"/>
+      <c r="K46" s="24"/>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
       <c r="N46" s="24"/>
@@ -5316,11 +5265,10 @@
       <c r="S46" s="24"/>
       <c r="T46" s="24"/>
       <c r="U46" s="24"/>
-      <c r="V46" s="24"/>
-      <c r="W46" s="25"/>
-      <c r="X46" s="17"/>
-    </row>
-    <row r="47" spans="1:24" thickBot="1">
+      <c r="V46" s="25"/>
+      <c r="W46" s="17"/>
+    </row>
+    <row r="47" spans="1:23" thickBot="1">
       <c r="A47" s="22">
         <v>46</v>
       </c>
@@ -5333,7 +5281,7 @@
       <c r="H47" s="24"/>
       <c r="I47" s="54"/>
       <c r="J47" s="24"/>
-      <c r="K47" s="54"/>
+      <c r="K47" s="24"/>
       <c r="L47" s="24"/>
       <c r="M47" s="24"/>
       <c r="N47" s="24"/>
@@ -5344,11 +5292,10 @@
       <c r="S47" s="24"/>
       <c r="T47" s="24"/>
       <c r="U47" s="24"/>
-      <c r="V47" s="24"/>
-      <c r="W47" s="25"/>
-      <c r="X47" s="17"/>
-    </row>
-    <row r="48" spans="1:24" thickBot="1">
+      <c r="V47" s="25"/>
+      <c r="W47" s="17"/>
+    </row>
+    <row r="48" spans="1:23" thickBot="1">
       <c r="A48" s="22">
         <v>47</v>
       </c>
@@ -5361,7 +5308,7 @@
       <c r="H48" s="24"/>
       <c r="I48" s="54"/>
       <c r="J48" s="24"/>
-      <c r="K48" s="54"/>
+      <c r="K48" s="24"/>
       <c r="L48" s="24"/>
       <c r="M48" s="24"/>
       <c r="N48" s="24"/>
@@ -5372,11 +5319,10 @@
       <c r="S48" s="24"/>
       <c r="T48" s="24"/>
       <c r="U48" s="24"/>
-      <c r="V48" s="24"/>
-      <c r="W48" s="25"/>
-      <c r="X48" s="17"/>
-    </row>
-    <row r="49" spans="1:24" thickBot="1">
+      <c r="V48" s="25"/>
+      <c r="W48" s="17"/>
+    </row>
+    <row r="49" spans="1:23" thickBot="1">
       <c r="A49" s="22">
         <v>48</v>
       </c>
@@ -5389,7 +5335,7 @@
       <c r="H49" s="24"/>
       <c r="I49" s="54"/>
       <c r="J49" s="24"/>
-      <c r="K49" s="54"/>
+      <c r="K49" s="24"/>
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
       <c r="N49" s="24"/>
@@ -5400,11 +5346,10 @@
       <c r="S49" s="24"/>
       <c r="T49" s="24"/>
       <c r="U49" s="24"/>
-      <c r="V49" s="24"/>
-      <c r="W49" s="25"/>
-      <c r="X49" s="17"/>
-    </row>
-    <row r="50" spans="1:24" thickBot="1">
+      <c r="V49" s="25"/>
+      <c r="W49" s="17"/>
+    </row>
+    <row r="50" spans="1:23" thickBot="1">
       <c r="A50" s="22">
         <v>49</v>
       </c>
@@ -5417,7 +5362,7 @@
       <c r="H50" s="24"/>
       <c r="I50" s="54"/>
       <c r="J50" s="24"/>
-      <c r="K50" s="54"/>
+      <c r="K50" s="24"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
@@ -5428,11 +5373,10 @@
       <c r="S50" s="24"/>
       <c r="T50" s="24"/>
       <c r="U50" s="24"/>
-      <c r="V50" s="24"/>
-      <c r="W50" s="25"/>
-      <c r="X50" s="17"/>
-    </row>
-    <row r="51" spans="1:24" thickBot="1">
+      <c r="V50" s="25"/>
+      <c r="W50" s="17"/>
+    </row>
+    <row r="51" spans="1:23" thickBot="1">
       <c r="A51" s="23">
         <v>50</v>
       </c>
@@ -5445,7 +5389,7 @@
       <c r="H51" s="26"/>
       <c r="I51" s="55"/>
       <c r="J51" s="26"/>
-      <c r="K51" s="55"/>
+      <c r="K51" s="26"/>
       <c r="L51" s="26"/>
       <c r="M51" s="26"/>
       <c r="N51" s="26"/>
@@ -5456,11 +5400,10 @@
       <c r="S51" s="26"/>
       <c r="T51" s="26"/>
       <c r="U51" s="26"/>
-      <c r="V51" s="26"/>
-      <c r="W51" s="27"/>
-      <c r="X51" s="17"/>
-    </row>
-    <row r="52" spans="1:24" ht="15" thickTop="1" thickBot="1">
+      <c r="V51" s="27"/>
+      <c r="W51" s="17"/>
+    </row>
+    <row r="52" spans="1:23" ht="15" thickTop="1" thickBot="1">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
@@ -5483,27 +5426,26 @@
       <c r="T52" s="18"/>
       <c r="U52" s="18"/>
       <c r="V52" s="18"/>
-      <c r="W52" s="18"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="17">
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the volume of fuel in liters used during this trip (0-1000)." sqref="O2:O51">
+  <dataValidations count="16">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the volume of fuel in liters used during this trip (0-1000)." sqref="N2:N51">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must indicate whether a sail was used on this trip. Permitted values are:_x000d__x000d_Y : Yes_x000d_N: N" sqref="N2:N51">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must indicate whether a sail was used on this trip. Permitted values are:_x000d__x000d_Y : Yes_x000d_N: N" sqref="M2:M51">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total number of people onboard during thsi trip (1-20)." sqref="P2:P51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total number of people onboard during thsi trip (1-20)." sqref="O2:O51">
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total number of fish landed (0-10000). Leave blank if not known." sqref="V2:V51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total number of fish landed (0-10000). Leave blank if not known." sqref="U2:U51">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total value of the catch in Rupia (0-100000000). Leave blank if not known." sqref="W2:W51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total value of the catch in Rupia (0-100000000). Leave blank if not known." sqref="V2:V51">
       <formula1>0</formula1>
       <formula2>100000000</formula2>
     </dataValidation>
@@ -5518,15 +5460,15 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid time." sqref="J2:J51 K3:K51">
+    <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid time." sqref="J2:J51">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total weight of the catch in kilograms (0-10000). Leave blank if not known." sqref="U2:U51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total weight of the catch in kilograms (0-10000). Leave blank if not known." sqref="T2:T51">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid arrival time that is after the departure time." sqref="L2:L51">
+    <dataValidation type="time" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid arrival time that is after the departure time." sqref="K2:K51">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>
@@ -5537,19 +5479,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="The following values are allowed:_x000d__x000d_OC - outrigger canoe" sqref="D2:D51">
       <formula1>"OC"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="Please select a value from the list:_x000d__x000d_0 = No fish caught_x000d_R = Rusak (mechanical problem)_x000d_H = Hilang (gear lost)_x000d_C = cuaca (bad weather)" sqref="M2:M51">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="Please select a value from the list:_x000d__x000d_0 = No fish caught_x000d_R = Rusak (mechanical problem)_x000d_H = Hilang (gear lost)_x000d_C = cuaca (bad weather)" sqref="L2:L51">
       <formula1>"0,R,H,C"</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the weight of ice in kg." sqref="R2:R51">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the weight of ice in kg." sqref="Q2:Q51">
       <formula1>0</formula1>
       <formula2>99</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a recognized code for the sea conditions. Permitted values are:_x000d__x000d_1: Calm_x000d_2: Moderate_x000d_3: Rough" sqref="S2:S51">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a recognized code for the sea conditions. Permitted values are:_x000d__x000d_1: Calm_x000d_2: Moderate_x000d_3: Rough" sqref="R2:R51">
       <formula1>"1,2,3"</formula1>
-    </dataValidation>
-    <dataValidation type="date" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid time." sqref="K2">
-      <formula1>I2</formula1>
-      <formula2>55153</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5567,13 +5505,13 @@
           <x14:formula1>
             <xm:f>'Gear Codes'!$A$2:$A$62</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q51</xm:sqref>
+          <xm:sqref>P2:P51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid fish ID code. Please check the &quot;Fish Codes&quot; tab.">
           <x14:formula1>
             <xm:f>'Species Codes'!A1:A1000</xm:f>
           </x14:formula1>
-          <xm:sqref>T2:T51</xm:sqref>
+          <xm:sqref>S2:S51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>